<commit_message>
Updated performance functions and class
</commit_message>
<xml_diff>
--- a/Polynomials.xlsx
+++ b/Polynomials.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbburf/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbburf/development - sw/sabine-basic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61EA04B7-2801-E84A-8F1E-333424DF0832}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1DF5A5E8-48DD-7C4E-AB52-B8FA212DFA6B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="660" windowWidth="28040" windowHeight="17040" xr2:uid="{290ACE22-76F4-C04C-A5BB-846EA80AA6F7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>I</t>
   </si>
@@ -33,13 +33,81 @@
     <t>Flux</t>
   </si>
   <si>
-    <t>Normalized(Flux)</t>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C0</t>
+  </si>
+  <si>
+    <t>Flux(Tj) - Normalized to Tj = 25</t>
+  </si>
+  <si>
+    <t>Flux(I) - Normalized to I = 900mA</t>
+  </si>
+  <si>
+    <t>Tj =&gt;</t>
+  </si>
+  <si>
+    <t>I =&gt;</t>
+  </si>
+  <si>
+    <t>Vf(I)</t>
+  </si>
+  <si>
+    <t>Vf(Tj)</t>
+  </si>
+  <si>
+    <t>Vf</t>
+  </si>
+  <si>
+    <t>Rth(I)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       </t>
+  </si>
+  <si>
+    <t>Normalized</t>
+  </si>
+  <si>
+    <t>R^2</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>I &amp; Tj</t>
+  </si>
+  <si>
+    <t>mV/DegC</t>
+  </si>
+  <si>
+    <t>DegC/Watt</t>
+  </si>
+  <si>
+    <t>Tc =&gt;</t>
+  </si>
+  <si>
+    <t>LN1</t>
+  </si>
+  <si>
+    <t>LN0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="180" formatCode="0.00000000000"/>
+    <numFmt numFmtId="189" formatCode="0.0000000000E+00"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -72,7 +140,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -80,12 +148,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -94,6 +171,26 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="189" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -126,37 +223,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -166,7 +233,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -198,28 +265,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="log"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="3"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.17821930243348105"/>
-                  <c:y val="-0.13329674492899052"/>
+                  <c:x val="-0.36238556788260329"/>
+                  <c:y val="2.7728602890155971E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="0.0000000000E+00" sourceLinked="0"/>
@@ -254,26 +306,23 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$8</c:f>
+              <c:f>Sheet1!$B$14:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>450</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>600</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>900</c:v>
+                  <c:v>1350</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1350</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>1800</c:v>
                 </c:pt>
               </c:numCache>
@@ -281,27 +330,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$8</c:f>
+              <c:f>Sheet1!$D$14:$D$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.95402298850574729</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.53700000000000003</c:v>
+                  <c:v>0.97701149425287359</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.70440000000000003</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.0229885057471266</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4874000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.9139999999999999</c:v>
+                  <c:v>1.0373563218390807</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1066,7 +1112,7 @@
       <xdr:rowOff>196850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1395,23 +1441,40 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90C48A5F-8F47-774A-8A09-6D1D5B804349}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:D8"/>
+  <dimension ref="B1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" customWidth="1"/>
+    <col min="6" max="6" width="103.83203125" customWidth="1"/>
+    <col min="7" max="7" width="6" customWidth="1"/>
+    <col min="8" max="8" width="6.33203125" customWidth="1"/>
+    <col min="9" max="9" width="6.5" customWidth="1"/>
+    <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D1">
+    <row r="1" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="1">
         <v>5000</v>
       </c>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1419,62 +1482,99 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="J2" s="13">
+        <v>2.121391239E-12</v>
+      </c>
+      <c r="L2" s="1">
+        <v>900</v>
+      </c>
+      <c r="M2" s="2">
+        <f>(J2*L2^3+J3*L2^2+J4*L2+J5)</f>
+        <v>1.0039830763274311</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <v>0</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="8">
         <v>0</v>
       </c>
       <c r="D3" s="2">
         <f>C3/D$1</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="13">
+        <v>-1.3267708046E-7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>450</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="8">
         <v>2685</v>
       </c>
       <c r="D4" s="2">
         <f>C4/D$1</f>
         <v>0.53700000000000003</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="I4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="13">
+        <v>1.2307082973E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>600</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="8">
         <v>3522</v>
       </c>
       <c r="D5" s="2">
         <f>C5/D$1</f>
         <v>0.70440000000000003</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="13">
+        <v>2.2675497168000002E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>900</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="8">
         <v>5000</v>
       </c>
       <c r="D6" s="2">
         <f>C6/D$1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="I6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="11">
+        <v>0.99976327267999998</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>1350</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="8">
         <v>7437</v>
       </c>
       <c r="D7" s="2">
@@ -1482,19 +1582,287 @@
         <v>1.4874000000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>1800</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="8">
         <v>9570</v>
       </c>
       <c r="D8" s="2">
         <f>C8/D$1</f>
         <v>1.9139999999999999</v>
       </c>
+      <c r="H8" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="6"/>
+      <c r="I9" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="13">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>25</v>
+      </c>
+      <c r="M9" s="2">
+        <f>J9*L9^3+J10*L9^2+J11*L9+J12</f>
+        <v>0.9999686274833125</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B10" s="1">
+        <v>950</v>
+      </c>
+      <c r="C10" s="8">
+        <f>D10*D1</f>
+        <v>5267.5909742509384</v>
+      </c>
+      <c r="D10" s="2">
+        <f>(J2*B10^3+J3*B10^2+J4*B10+J5)</f>
+        <v>1.0535181948501877</v>
+      </c>
+      <c r="I10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" s="13">
+        <v>-2.0168067226999998E-6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="I11" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="13">
+        <v>-1.5188515406E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="D12" s="1">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="I12" t="s">
+        <v>5</v>
+      </c>
+      <c r="J12" s="13">
+        <v>1.0392004202</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="11"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>450</v>
+      </c>
+      <c r="C14">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="D14" s="2">
+        <f>C14/D$12</f>
+        <v>0.95402298850574729</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>600</v>
+      </c>
+      <c r="C15">
+        <v>34</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" ref="D15:D18" si="0">C15/D$12</f>
+        <v>0.97701149425287359</v>
+      </c>
+      <c r="H15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="M15" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>900</v>
+      </c>
+      <c r="C16">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="13">
+        <v>5.9241490564999999E-2</v>
+      </c>
+      <c r="L16" s="1">
+        <v>900</v>
+      </c>
+      <c r="M16" s="2">
+        <f>J16*LN(L16)+J17</f>
+        <v>0.99827586207088248</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>1350</v>
+      </c>
+      <c r="C17">
+        <v>35.6</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0229885057471266</v>
+      </c>
+      <c r="I17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J17" s="13">
+        <v>0.59529185687999997</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>1800</v>
+      </c>
+      <c r="C18">
+        <v>36.1</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0373563218390807</v>
+      </c>
+      <c r="I18" t="s">
+        <v>16</v>
+      </c>
+      <c r="J18">
+        <v>0.99450000000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>11</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="M20" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="I21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="5">
+        <v>-14.9</v>
+      </c>
+      <c r="K21" t="s">
+        <v>19</v>
+      </c>
+      <c r="L21" s="1">
+        <v>105</v>
+      </c>
+      <c r="M21" s="10">
+        <f>(L21-25)*J21/1000</f>
+        <v>-1.1919999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="I22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>13</v>
+      </c>
+      <c r="L24" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M24" s="12"/>
+    </row>
+    <row r="25" spans="2:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="I25" t="s">
+        <v>17</v>
+      </c>
+      <c r="J25">
+        <v>0.15</v>
+      </c>
+      <c r="K25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L25" s="1">
+        <v>1800</v>
+      </c>
+      <c r="M25" s="10">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="I26" t="s">
+        <v>16</v>
+      </c>
+      <c r="J26" s="11">
+        <v>1</v>
+      </c>
+      <c r="K26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="J27" s="4"/>
+      <c r="K27" t="s">
+        <v>14</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M27" s="7">
+        <f>(M25+(J25*(L25/1000)*D12*(J16*LN(L25)+J17)))</f>
+        <v>114.76562862600798</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="M31" s="8"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="L24:M24"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Updated relationships + added logic for temp toggle
</commit_message>
<xml_diff>
--- a/Polynomials.xlsx
+++ b/Polynomials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbburf/development - sw/sabine-basic/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/development-sw/sabine-basic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1DF5A5E8-48DD-7C4E-AB52-B8FA212DFA6B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CC0DE067-9D13-6D4C-AF55-F91B99155127}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="660" windowWidth="28040" windowHeight="17040" xr2:uid="{290ACE22-76F4-C04C-A5BB-846EA80AA6F7}"/>
+    <workbookView xWindow="640" yWindow="800" windowWidth="28040" windowHeight="17040" xr2:uid="{290ACE22-76F4-C04C-A5BB-846EA80AA6F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -104,9 +104,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="171" formatCode="0.0"/>
-    <numFmt numFmtId="180" formatCode="0.00000000000"/>
-    <numFmt numFmtId="189" formatCode="0.0000000000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.00000000000"/>
+    <numFmt numFmtId="166" formatCode="0.0000000000E+00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -174,7 +174,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -186,11 +186,11 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="189" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1487,7 +1487,7 @@
       <c r="I2" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="13">
+      <c r="J2" s="12">
         <v>2.121391239E-12</v>
       </c>
       <c r="L2" s="1">
@@ -1506,13 +1506,13 @@
         <v>0</v>
       </c>
       <c r="D3" s="2">
-        <f>C3/D$1</f>
+        <f t="shared" ref="D3:D8" si="0">C3/D$1</f>
         <v>0</v>
       </c>
       <c r="I3" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="12">
         <v>-1.3267708046E-7</v>
       </c>
     </row>
@@ -1524,13 +1524,13 @@
         <v>2685</v>
       </c>
       <c r="D4" s="2">
-        <f>C4/D$1</f>
+        <f t="shared" si="0"/>
         <v>0.53700000000000003</v>
       </c>
       <c r="I4" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="12">
         <v>1.2307082973E-3</v>
       </c>
     </row>
@@ -1542,13 +1542,13 @@
         <v>3522</v>
       </c>
       <c r="D5" s="2">
-        <f>C5/D$1</f>
+        <f t="shared" si="0"/>
         <v>0.70440000000000003</v>
       </c>
       <c r="I5" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="12">
         <v>2.2675497168000002E-3</v>
       </c>
     </row>
@@ -1560,7 +1560,7 @@
         <v>5000</v>
       </c>
       <c r="D6" s="2">
-        <f>C6/D$1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I6" t="s">
@@ -1578,7 +1578,7 @@
         <v>7437</v>
       </c>
       <c r="D7" s="2">
-        <f>C7/D$1</f>
+        <f t="shared" si="0"/>
         <v>1.4874000000000001</v>
       </c>
     </row>
@@ -1590,7 +1590,7 @@
         <v>9570</v>
       </c>
       <c r="D8" s="2">
-        <f>C8/D$1</f>
+        <f t="shared" si="0"/>
         <v>1.9139999999999999</v>
       </c>
       <c r="H8" t="s">
@@ -1608,7 +1608,7 @@
       <c r="I9" t="s">
         <v>2</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="12">
         <v>0</v>
       </c>
       <c r="L9" s="1">
@@ -1634,7 +1634,7 @@
       <c r="I10" t="s">
         <v>3</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="12">
         <v>-2.0168067226999998E-6</v>
       </c>
     </row>
@@ -1642,7 +1642,7 @@
       <c r="I11" t="s">
         <v>4</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="12">
         <v>-1.5188515406E-3</v>
       </c>
     </row>
@@ -1653,7 +1653,7 @@
       <c r="I12" t="s">
         <v>5</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="12">
         <v>1.0392004202</v>
       </c>
     </row>
@@ -1692,7 +1692,7 @@
         <v>34</v>
       </c>
       <c r="D15" s="2">
-        <f t="shared" ref="D15:D18" si="0">C15/D$12</f>
+        <f t="shared" ref="D15:D18" si="1">C15/D$12</f>
         <v>0.97701149425287359</v>
       </c>
       <c r="H15" t="s">
@@ -1713,21 +1713,21 @@
         <v>34.799999999999997</v>
       </c>
       <c r="D16" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I16" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="13">
+      <c r="J16" s="12">
         <v>5.9241490564999999E-2</v>
       </c>
       <c r="L16" s="1">
-        <v>900</v>
+        <v>600</v>
       </c>
       <c r="M16" s="2">
         <f>J16*LN(L16)+J17</f>
-        <v>0.99827586207088248</v>
+        <v>0.97425550469445599</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.2">
@@ -1738,13 +1738,13 @@
         <v>35.6</v>
       </c>
       <c r="D17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0229885057471266</v>
       </c>
       <c r="I17" t="s">
         <v>23</v>
       </c>
-      <c r="J17" s="13">
+      <c r="J17" s="12">
         <v>0.59529185687999997</v>
       </c>
     </row>
@@ -1756,7 +1756,7 @@
         <v>36.1</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0373563218390807</v>
       </c>
       <c r="I18" t="s">
@@ -1810,10 +1810,10 @@
       <c r="H24" t="s">
         <v>13</v>
       </c>
-      <c r="L24" s="12" t="s">
+      <c r="L24" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="M24" s="12"/>
+      <c r="M24" s="13"/>
     </row>
     <row r="25" spans="2:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="I25" t="s">

</xml_diff>